<commit_message>
Added most instructions to interpreter
</commit_message>
<xml_diff>
--- a/doc/instructionset.xlsx
+++ b/doc/instructionset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kholisa32\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11EECD6-2789-4220-8009-2798FDE88F78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C67244-9EDC-4834-BD81-2B0B2F315064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="122">
   <si>
     <t>Mnemonic</t>
   </si>
@@ -378,13 +378,19 @@
     <t>DJNZ Rn, label</t>
   </si>
   <si>
-    <t>DJZ Rn label</t>
-  </si>
-  <si>
     <t>0xA3nnuuuu</t>
   </si>
   <si>
     <t>Transmits a string over the UART (max 256 chars)</t>
+  </si>
+  <si>
+    <t>DJZ Rn, label</t>
+  </si>
+  <si>
+    <t>Bitwise AND, OR, XOR, COMP to be added</t>
+  </si>
+  <si>
+    <t>PUSH and POP to be added</t>
   </si>
 </sst>
 </file>
@@ -567,11 +573,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1359,7 +1365,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>86</v>
@@ -1375,6 +1381,16 @@
       </c>
       <c r="C53" s="11"/>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>121</v>
+      </c>
+    </row>
     <row r="61" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
@@ -1405,52 +1421,62 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="19" t="s">
+    <row r="65" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="21" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C66" s="20" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="12"/>
       <c r="B67" s="2" t="s">
         <v>104</v>
       </c>
+      <c r="C67" s="13"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B68" s="23" t="s">
+      <c r="A68" s="12"/>
+      <c r="B68" s="24" t="s">
         <v>105</v>
       </c>
+      <c r="C68" s="13"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B69" s="24" t="s">
+      <c r="A69" s="12"/>
+      <c r="B69" s="23" t="s">
         <v>105</v>
       </c>
+      <c r="C69" s="13"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="24" t="s">
+      <c r="A70" s="12"/>
+      <c r="B70" s="23" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
+      <c r="C70" s="13"/>
+    </row>
+    <row r="71" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="9"/>
+      <c r="B71" s="10" t="s">
         <v>104</v>
       </c>
+      <c r="C71" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>